<commit_message>
Added all the diagrams
</commit_message>
<xml_diff>
--- a/tab.xlsx
+++ b/tab.xlsx
@@ -16,30 +16,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Typ diagramu</t>
   </si>
   <si>
-    <t>Využitie</t>
+    <t>Knihy spolu</t>
+  </si>
+  <si>
+    <t>Nástroje</t>
+  </si>
+  <si>
+    <t>Kurzy</t>
+  </si>
+  <si>
+    <t>Tutoriály</t>
+  </si>
+  <si>
+    <t>Všetky materiály</t>
+  </si>
+  <si>
+    <t>Knižné návody</t>
+  </si>
+  <si>
+    <t>Knižné špecifikácie</t>
+  </si>
+  <si>
+    <t>Triedny</t>
+  </si>
+  <si>
+    <t>Komponentový</t>
+  </si>
+  <si>
+    <t>Diagram nasadenia</t>
+  </si>
+  <si>
+    <t>Objektový</t>
+  </si>
+  <si>
+    <t>Balíkový</t>
+  </si>
+  <si>
+    <t>Činnostný</t>
   </si>
   <si>
     <t>Sekvenčný</t>
   </si>
   <si>
+    <t>Komunikačný</t>
+  </si>
+  <si>
+    <t>Interakčný</t>
+  </si>
+  <si>
+    <t>Časový</t>
+  </si>
+  <si>
+    <t>Diagram prípadu použitia</t>
+  </si>
+  <si>
     <t>Stavový</t>
   </si>
   <si>
-    <t>Objektový</t>
-  </si>
-  <si>
-    <t>Triedny</t>
-  </si>
-  <si>
-    <t>Činnostný</t>
-  </si>
-  <si>
-    <t>Prípadu použitia</t>
+    <t>Profilový</t>
+  </si>
+  <si>
+    <t>Kompozitný</t>
   </si>
 </sst>
 </file>
@@ -65,12 +107,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,79 +135,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -460,73 +442,409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C8"/>
+  <dimension ref="C3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B2" s="7" t="s">
+    <row r="3" spans="3:10">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
+    </row>
+    <row r="4" spans="3:10">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
         <v>0.98</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
+    <row r="11" spans="3:10">
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.93</v>
+      </c>
+      <c r="F11" s="5">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10">
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10">
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J15" s="3">
         <v>0.96</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
+    <row r="16" spans="3:10">
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J16" s="3">
         <v>0.96</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.71</v>
+    <row r="17" spans="3:10">
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>